<commit_message>
Removed spaces from headers
</commit_message>
<xml_diff>
--- a/sample_data/DataFile.xlsx
+++ b/sample_data/DataFile.xlsx
@@ -69,15 +69,9 @@
     <t>Midcall</t>
   </si>
   <si>
-    <t>Clinic Group</t>
-  </si>
-  <si>
     <t>Clinic</t>
   </si>
   <si>
-    <t>Number of Residents</t>
-  </si>
-  <si>
     <t>Purple</t>
   </si>
   <si>
@@ -99,15 +93,6 @@
     <t>Orange</t>
   </si>
   <si>
-    <t>RESIDENT ID</t>
-  </si>
-  <si>
-    <t>Clinic Groups</t>
-  </si>
-  <si>
-    <t>Year Level</t>
-  </si>
-  <si>
     <t>CardFloor</t>
   </si>
   <si>
@@ -123,163 +108,178 @@
     <t>VAC</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 5</t>
-  </si>
-  <si>
-    <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
-  </si>
-  <si>
-    <t>Week 8</t>
-  </si>
-  <si>
-    <t>Week 9</t>
-  </si>
-  <si>
-    <t>Week 10</t>
-  </si>
-  <si>
-    <t>Week 11</t>
-  </si>
-  <si>
-    <t>Week 12</t>
-  </si>
-  <si>
-    <t>Week 13</t>
-  </si>
-  <si>
-    <t>Week 14</t>
-  </si>
-  <si>
-    <t>Week 15</t>
-  </si>
-  <si>
-    <t>Week 16</t>
-  </si>
-  <si>
-    <t>Week 17</t>
-  </si>
-  <si>
-    <t>Week 18</t>
-  </si>
-  <si>
-    <t>Week 19</t>
-  </si>
-  <si>
-    <t>Week 20</t>
-  </si>
-  <si>
-    <t>Week 21</t>
-  </si>
-  <si>
-    <t>Week 22</t>
-  </si>
-  <si>
-    <t>Week 23</t>
-  </si>
-  <si>
-    <t>Week 24</t>
-  </si>
-  <si>
-    <t>Week 25</t>
-  </si>
-  <si>
-    <t>Week 26</t>
-  </si>
-  <si>
-    <t>Week 27</t>
-  </si>
-  <si>
-    <t>Week 28</t>
-  </si>
-  <si>
-    <t>Week 29</t>
-  </si>
-  <si>
-    <t>Week 30</t>
-  </si>
-  <si>
-    <t>Week 31</t>
-  </si>
-  <si>
-    <t>Week 32</t>
-  </si>
-  <si>
-    <t>Week 33</t>
-  </si>
-  <si>
-    <t>Week 34</t>
-  </si>
-  <si>
-    <t>Week 35</t>
-  </si>
-  <si>
-    <t>Week 36</t>
-  </si>
-  <si>
-    <t>Week 37</t>
-  </si>
-  <si>
-    <t>Week 38</t>
-  </si>
-  <si>
-    <t>Week 39</t>
-  </si>
-  <si>
-    <t>Week 40</t>
-  </si>
-  <si>
-    <t>Week 41</t>
-  </si>
-  <si>
-    <t>Week 42</t>
-  </si>
-  <si>
-    <t>Week 43</t>
-  </si>
-  <si>
-    <t>Week 44</t>
-  </si>
-  <si>
-    <t>Week 45</t>
-  </si>
-  <si>
-    <t>Week 46</t>
-  </si>
-  <si>
-    <t>Week 47</t>
-  </si>
-  <si>
-    <t>Week 48</t>
-  </si>
-  <si>
-    <t>Week 49</t>
-  </si>
-  <si>
-    <t>Week 50</t>
-  </si>
-  <si>
-    <t>Week 51</t>
-  </si>
-  <si>
-    <t>Week 52</t>
-  </si>
-  <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Resident_ID</t>
+  </si>
+  <si>
+    <t>Year_Level</t>
+  </si>
+  <si>
+    <t>Week_1</t>
+  </si>
+  <si>
+    <t>Week_2</t>
+  </si>
+  <si>
+    <t>Week_3</t>
+  </si>
+  <si>
+    <t>Week_4</t>
+  </si>
+  <si>
+    <t>Week_5</t>
+  </si>
+  <si>
+    <t>Week_6</t>
+  </si>
+  <si>
+    <t>Week_7</t>
+  </si>
+  <si>
+    <t>Week_8</t>
+  </si>
+  <si>
+    <t>Week_9</t>
+  </si>
+  <si>
+    <t>Week_10</t>
+  </si>
+  <si>
+    <t>Week_11</t>
+  </si>
+  <si>
+    <t>Week_12</t>
+  </si>
+  <si>
+    <t>Week_13</t>
+  </si>
+  <si>
+    <t>Week_14</t>
+  </si>
+  <si>
+    <t>Week_15</t>
+  </si>
+  <si>
+    <t>Week_16</t>
+  </si>
+  <si>
+    <t>Week_17</t>
+  </si>
+  <si>
+    <t>Week_18</t>
+  </si>
+  <si>
+    <t>Week_19</t>
+  </si>
+  <si>
+    <t>Week_20</t>
+  </si>
+  <si>
+    <t>Week_21</t>
+  </si>
+  <si>
+    <t>Week_22</t>
+  </si>
+  <si>
+    <t>Week_23</t>
+  </si>
+  <si>
+    <t>Week_24</t>
+  </si>
+  <si>
+    <t>Week_25</t>
+  </si>
+  <si>
+    <t>Week_26</t>
+  </si>
+  <si>
+    <t>Week_27</t>
+  </si>
+  <si>
+    <t>Week_28</t>
+  </si>
+  <si>
+    <t>Week_29</t>
+  </si>
+  <si>
+    <t>Week_30</t>
+  </si>
+  <si>
+    <t>Week_31</t>
+  </si>
+  <si>
+    <t>Week_32</t>
+  </si>
+  <si>
+    <t>Week_33</t>
+  </si>
+  <si>
+    <t>Week_34</t>
+  </si>
+  <si>
+    <t>Week_35</t>
+  </si>
+  <si>
+    <t>Week_36</t>
+  </si>
+  <si>
+    <t>Week_37</t>
+  </si>
+  <si>
+    <t>Week_38</t>
+  </si>
+  <si>
+    <t>Week_39</t>
+  </si>
+  <si>
+    <t>Week_40</t>
+  </si>
+  <si>
+    <t>Week_41</t>
+  </si>
+  <si>
+    <t>Week_42</t>
+  </si>
+  <si>
+    <t>Week_43</t>
+  </si>
+  <si>
+    <t>Week_44</t>
+  </si>
+  <si>
+    <t>Week_45</t>
+  </si>
+  <si>
+    <t>Week_46</t>
+  </si>
+  <si>
+    <t>Week_47</t>
+  </si>
+  <si>
+    <t>Week_48</t>
+  </si>
+  <si>
+    <t>Week_49</t>
+  </si>
+  <si>
+    <t>Week_50</t>
+  </si>
+  <si>
+    <t>Week_51</t>
+  </si>
+  <si>
+    <t>Week_52</t>
+  </si>
+  <si>
+    <t>Clinic_Group</t>
+  </si>
+  <si>
+    <t>Number_of_Residents</t>
+  </si>
+  <si>
+    <t>Clinic_Groups</t>
   </si>
 </sst>
 </file>
@@ -392,99 +392,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -822,7 +730,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -838,13 +746,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
@@ -852,10 +760,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5">
         <f>COUNTIF(Parameters!$B:$B,"Purple")</f>
@@ -867,10 +775,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="5">
         <f>COUNTIF(Parameters!$B:$B,"Yellow")</f>
@@ -882,10 +790,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="5">
         <f>COUNTIF(Parameters!$B:$B,"Blue")</f>
@@ -897,10 +805,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5">
         <f>COUNTIF(Parameters!$B:$B,"Green")</f>
@@ -912,10 +820,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5">
         <f>COUNTIF(Parameters!$B:$B,"Orange")</f>
@@ -977,14 +885,14 @@
   <dimension ref="A1:BN58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.0625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.3125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.875" bestFit="1" customWidth="1"/>
@@ -996,28 +904,28 @@
     <col min="12" max="12" width="4.4375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.8125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.8125" bestFit="1" customWidth="1"/>
-    <col min="15" max="23" width="6.4375" bestFit="1" customWidth="1"/>
-    <col min="24" max="66" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="23" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="66" width="7.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -1029,175 +937,175 @@
         <v>2</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="BM1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BN1" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.5">
@@ -1205,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -1329,7 +1237,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -1455,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1605,7 +1513,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1731,7 +1639,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1891,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1955,7 +1863,7 @@
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="5" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="AO7" s="5">
         <v>7</v>
@@ -2005,7 +1913,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -2071,7 +1979,7 @@
         <v>4</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="AC8" s="5"/>
       <c r="AD8" s="5"/>
@@ -2123,7 +2031,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -2251,7 +2159,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -2395,7 +2303,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -2527,7 +2435,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -2639,7 +2547,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -2771,7 +2679,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -2897,7 +2805,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -3007,7 +2915,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -3135,7 +3043,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -3255,7 +3163,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -3365,7 +3273,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -3477,7 +3385,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -3573,7 +3481,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21" s="5">
         <v>2</v>
@@ -3677,7 +3585,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C22" s="5">
         <v>2</v>
@@ -3799,7 +3707,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="5">
         <v>2</v>
@@ -3923,7 +3831,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" s="5">
         <v>2</v>
@@ -4027,7 +3935,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="5">
         <v>2</v>
@@ -4139,7 +4047,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26" s="5">
         <v>2</v>
@@ -4267,7 +4175,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C27" s="5">
         <v>2</v>
@@ -4395,7 +4303,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="5">
         <v>2</v>
@@ -4499,7 +4407,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" s="5">
         <v>2</v>
@@ -4607,7 +4515,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C30" s="5">
         <v>2</v>
@@ -4719,7 +4627,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C31" s="5">
         <v>2</v>
@@ -4853,7 +4761,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C32" s="5">
         <v>2</v>
@@ -4981,7 +4889,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C33" s="5">
         <v>2</v>
@@ -5105,7 +5013,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C34" s="5">
         <v>2</v>
@@ -5245,7 +5153,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C35" s="5">
         <v>2</v>
@@ -5347,7 +5255,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C36" s="5">
         <v>2</v>
@@ -5457,7 +5365,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C37" s="5">
         <v>2</v>
@@ -5587,7 +5495,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C38" s="5">
         <v>2</v>
@@ -5709,7 +5617,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C39" s="5">
         <v>2</v>
@@ -5861,7 +5769,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C40" s="5">
         <v>3</v>
@@ -5973,7 +5881,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C41" s="5">
         <v>3</v>
@@ -6083,7 +5991,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C42" s="5">
         <v>3</v>
@@ -6148,7 +6056,7 @@
       <c r="AM42" s="5"/>
       <c r="AN42" s="5"/>
       <c r="AO42" s="5" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="AP42" s="5">
         <v>7</v>
@@ -6205,7 +6113,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C43" s="5">
         <v>3</v>
@@ -6317,7 +6225,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C44" s="5">
         <v>3</v>
@@ -6459,7 +6367,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C45" s="5">
         <v>3</v>
@@ -6563,7 +6471,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C46" s="5">
         <v>3</v>
@@ -6691,7 +6599,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C47" s="5">
         <v>3</v>
@@ -6797,7 +6705,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C48" s="5">
         <v>3</v>
@@ -6905,7 +6813,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C49" s="5">
         <v>3</v>
@@ -7029,7 +6937,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C50" s="5">
         <v>3</v>
@@ -7155,7 +7063,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C51" s="5">
         <v>3</v>
@@ -7261,7 +7169,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C52" s="5">
         <v>3</v>
@@ -7369,7 +7277,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C53" s="5">
         <v>3</v>
@@ -7481,7 +7389,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C54" s="5">
         <v>3</v>
@@ -7581,7 +7489,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C55" s="5">
         <v>3</v>
@@ -7622,16 +7530,16 @@
       <c r="Q55" s="5"/>
       <c r="R55" s="5"/>
       <c r="S55" s="5" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="U55" s="5" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="V55" s="5" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="W55" s="5">
         <v>7</v>
@@ -7703,7 +7611,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C56" s="5">
         <v>3</v>
@@ -7827,7 +7735,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C57" s="5">
         <v>3</v>
@@ -7929,7 +7837,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C58" s="5">
         <v>3</v>

</xml_diff>

<commit_message>
Added unit req's from paper
</commit_message>
<xml_diff>
--- a/sample_data/DataFile.xlsx
+++ b/sample_data/DataFile.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
-    <sheet name="Parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="Unit definitions" sheetId="3" r:id="rId2"/>
+    <sheet name="Parameters" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="106">
   <si>
     <t>Units</t>
   </si>
@@ -280,6 +281,69 @@
   </si>
   <si>
     <t>Clinic_Groups</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>R1Min</t>
+  </si>
+  <si>
+    <t>R1Max</t>
+  </si>
+  <si>
+    <t>R2Min</t>
+  </si>
+  <si>
+    <t>R2Max</t>
+  </si>
+  <si>
+    <t>R3Min</t>
+  </si>
+  <si>
+    <t>R3Max</t>
+  </si>
+  <si>
+    <t>R1F</t>
+  </si>
+  <si>
+    <t>HemeF</t>
+  </si>
+  <si>
+    <t>CardF</t>
+  </si>
+  <si>
+    <t>FloatF</t>
+  </si>
+  <si>
+    <t>mat_D</t>
+  </si>
+  <si>
+    <t>unlimited</t>
+  </si>
+  <si>
+    <t>MAT N</t>
+  </si>
+  <si>
+    <t>Sick call</t>
+  </si>
+  <si>
+    <t>Twig</t>
+  </si>
+  <si>
+    <t>Duration_Min</t>
+  </si>
+  <si>
+    <t>Duration_Max</t>
+  </si>
+  <si>
+    <t>Rotation_Min</t>
+  </si>
+  <si>
+    <t>Rotation_Max</t>
+  </si>
+  <si>
+    <t>Student_Req</t>
   </si>
 </sst>
 </file>
@@ -730,7 +794,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -882,9 +946,755 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="12.0625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed "unlimited" to 1000 since numbers and strings don't math together well
</commit_message>
<xml_diff>
--- a/sample_data/DataFile.xlsx
+++ b/sample_data/DataFile.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-443" windowWidth="25598" windowHeight="15998" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-443" windowWidth="25598" windowHeight="15998" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
     <sheet name="Unit definitions" sheetId="3" r:id="rId2"/>
     <sheet name="Parameters" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
   <si>
     <t>Units</t>
   </si>
@@ -317,9 +317,6 @@
   </si>
   <si>
     <t>mat_D</t>
-  </si>
-  <si>
-    <t>unlimited</t>
   </si>
   <si>
     <t>MAT N</t>
@@ -948,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -966,19 +963,19 @@
         <v>85</v>
       </c>
       <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>102</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>103</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>104</v>
-      </c>
-      <c r="F1" t="s">
-        <v>105</v>
       </c>
       <c r="G1" t="s">
         <v>86</v>
@@ -1242,8 +1239,8 @@
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
-        <v>97</v>
+      <c r="E8">
+        <v>1000</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -1269,7 +1266,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1280,8 +1277,8 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>97</v>
+      <c r="E9">
+        <v>1000</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -1318,8 +1315,8 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>97</v>
+      <c r="E10">
+        <v>1000</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -1327,20 +1324,20 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
-        <v>97</v>
+      <c r="H10">
+        <v>1000</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10" t="s">
-        <v>97</v>
+      <c r="J10">
+        <v>1000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
-      <c r="L10" t="s">
-        <v>97</v>
+      <c r="L10">
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.5">
@@ -1497,7 +1494,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1508,8 +1505,8 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>97</v>
+      <c r="E15">
+        <v>1000</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -1517,20 +1514,20 @@
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15" t="s">
-        <v>97</v>
+      <c r="H15">
+        <v>1000</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>97</v>
+      <c r="J15">
+        <v>1000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15" t="s">
-        <v>97</v>
+      <c r="L15">
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.5">
@@ -1611,7 +1608,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1694,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="O2:BN58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Added Hypothetical Unit types, day/night units, round 1 units
</commit_message>
<xml_diff>
--- a/sample_data/DataFile.xlsx
+++ b/sample_data/DataFile.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="113">
   <si>
     <t>Units</t>
   </si>
@@ -316,12 +316,6 @@
     <t>FloatF</t>
   </si>
   <si>
-    <t>mat_D</t>
-  </si>
-  <si>
-    <t>MAT N</t>
-  </si>
-  <si>
     <t>Sick call</t>
   </si>
   <si>
@@ -341,6 +335,36 @@
   </si>
   <si>
     <t>Student_Req</t>
+  </si>
+  <si>
+    <t>Unit_type</t>
+  </si>
+  <si>
+    <t>Day_Night</t>
+  </si>
+  <si>
+    <t>Night</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>round_1</t>
+  </si>
+  <si>
+    <t>Inpatient</t>
+  </si>
+  <si>
+    <t>Ambulatory</t>
+  </si>
+  <si>
+    <t>Elective</t>
+  </si>
+  <si>
+    <t>Vacation</t>
+  </si>
+  <si>
+    <t>Sick</t>
   </si>
 </sst>
 </file>
@@ -943,281 +967,336 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="12.0625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.0625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>85</v>
       </c>
       <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>87</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>89</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>90</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2" t="b">
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>2</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3" t="b">
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="I4" t="b">
         <v>1</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>94</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="b">
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="b">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
         <v>1</v>
       </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>95</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="b">
         <v>1</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>2</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="b">
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1225,33 +1304,42 @@
       <c r="L7">
         <v>1</v>
       </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
         <v>2</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>1000</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="b">
         <v>1</v>
       </c>
       <c r="J8">
@@ -1261,424 +1349,579 @@
         <v>1</v>
       </c>
       <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
         <v>1</v>
       </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="C9">
+      <c r="F9">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="H9">
         <v>1000</v>
       </c>
-      <c r="F9" t="b">
+      <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1000</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
+      <c r="F10">
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>1000</v>
       </c>
-      <c r="I10">
-        <v>0</v>
+      <c r="I10" t="b">
+        <v>1</v>
       </c>
       <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>1000</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>1000</v>
       </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1000</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B11">
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="C11">
+      <c r="F12">
         <v>2</v>
       </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>4</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>2</v>
       </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>5</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12" t="b">
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13" t="b">
         <v>1</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>2</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <v>1</v>
       </c>
-      <c r="L12">
+      <c r="O13">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="C13">
+      <c r="F14">
         <v>2</v>
       </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
       <c r="G14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" t="b">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
         <v>2</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>1000</v>
       </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>1000</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
         <v>1000</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B16">
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
         <v>2</v>
       </c>
-      <c r="C16">
+      <c r="F17">
         <v>2</v>
       </c>
-      <c r="D16">
+      <c r="G17">
         <v>2</v>
       </c>
-      <c r="E16">
+      <c r="H17">
         <v>8</v>
       </c>
-      <c r="F16" t="b">
+      <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="G16">
+      <c r="J17">
         <v>2</v>
       </c>
-      <c r="H16">
+      <c r="K17">
         <v>2</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18" t="b">
         <v>1</v>
       </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18">
-        <v>11</v>
-      </c>
-      <c r="F18" t="b">
+      <c r="J18">
         <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>2</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>11</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
         <v>2</v>
       </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A19" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B19">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="D19">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
         <v>10</v>
       </c>
-      <c r="E19">
+      <c r="H20">
         <v>11</v>
       </c>
-      <c r="F19" t="b">
+      <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="G19">
+      <c r="J20">
         <v>1</v>
       </c>
-      <c r="H19">
+      <c r="K20">
         <v>3</v>
       </c>
-      <c r="I19">
+      <c r="L20">
         <v>1</v>
       </c>
-      <c r="J19">
+      <c r="M20">
         <v>2</v>
       </c>
-      <c r="K19">
+      <c r="N20">
         <v>1</v>
       </c>
-      <c r="L19">
+      <c r="O20">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Redefined model.U to be a union of the other sets. And defined Ri to make separate the residents by year.
</commit_message>
<xml_diff>
--- a/sample_data/DataFile.xlsx
+++ b/sample_data/DataFile.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="112">
   <si>
     <t>Units</t>
   </si>
@@ -362,9 +362,6 @@
   </si>
   <si>
     <t>Vacation</t>
-  </si>
-  <si>
-    <t>Sick</t>
   </si>
 </sst>
 </file>
@@ -969,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1648,7 +1645,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
         <v>106</v>
@@ -1695,7 +1692,7 @@
         <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Finished importing sets! and updated excel file to fix issue with interpreting TRUE/FALSE in Pandas
</commit_message>
<xml_diff>
--- a/sample_data/DataFile.xlsx
+++ b/sample_data/DataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-443" windowWidth="25598" windowHeight="15998" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-443" windowWidth="13680" windowHeight="10500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="114">
   <si>
     <t>Units</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Vacation</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -966,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1037,8 +1043,8 @@
       <c r="C2" t="s">
         <v>106</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="s">
+        <v>112</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1052,9 +1058,8 @@
       <c r="H2">
         <v>4</v>
       </c>
-      <c r="I2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="I2" t="s">
+        <v>112</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1085,8 +1090,8 @@
       <c r="C3" t="s">
         <v>106</v>
       </c>
-      <c r="D3">
-        <v>0</v>
+      <c r="D3" t="s">
+        <v>112</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1100,9 +1105,8 @@
       <c r="H3">
         <v>4</v>
       </c>
-      <c r="I3" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+      <c r="I3" t="s">
+        <v>113</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1133,8 +1137,8 @@
       <c r="C4" t="s">
         <v>106</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>112</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1148,8 +1152,8 @@
       <c r="H4">
         <v>4</v>
       </c>
-      <c r="I4" t="b">
-        <v>1</v>
+      <c r="I4" t="s">
+        <v>113</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1180,8 +1184,8 @@
       <c r="C5" t="s">
         <v>106</v>
       </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="D5" t="s">
+        <v>112</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1195,8 +1199,8 @@
       <c r="H5">
         <v>4</v>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
+      <c r="I5" t="s">
+        <v>113</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1227,8 +1231,8 @@
       <c r="C6" t="s">
         <v>106</v>
       </c>
-      <c r="D6">
-        <v>0</v>
+      <c r="D6" t="s">
+        <v>112</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1242,8 +1246,8 @@
       <c r="H6">
         <v>4</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
+      <c r="I6" t="s">
+        <v>113</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1274,8 +1278,8 @@
       <c r="C7" t="s">
         <v>106</v>
       </c>
-      <c r="D7">
-        <v>0</v>
+      <c r="D7" t="s">
+        <v>112</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1289,8 +1293,8 @@
       <c r="H7">
         <v>4</v>
       </c>
-      <c r="I7" t="b">
-        <v>1</v>
+      <c r="I7" t="s">
+        <v>113</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1321,8 +1325,8 @@
       <c r="C8" t="s">
         <v>106</v>
       </c>
-      <c r="D8">
-        <v>0</v>
+      <c r="D8" t="s">
+        <v>112</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1336,8 +1340,8 @@
       <c r="H8">
         <v>4</v>
       </c>
-      <c r="I8" t="b">
-        <v>1</v>
+      <c r="I8" t="s">
+        <v>113</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1368,8 +1372,8 @@
       <c r="C9" t="s">
         <v>106</v>
       </c>
-      <c r="D9">
-        <v>0</v>
+      <c r="D9" t="s">
+        <v>112</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1383,8 +1387,8 @@
       <c r="H9">
         <v>1000</v>
       </c>
-      <c r="I9" t="b">
-        <v>1</v>
+      <c r="I9" t="s">
+        <v>113</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1415,8 +1419,8 @@
       <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="D10">
-        <v>0</v>
+      <c r="D10" t="s">
+        <v>112</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1430,8 +1434,8 @@
       <c r="H10">
         <v>1000</v>
       </c>
-      <c r="I10" t="b">
-        <v>1</v>
+      <c r="I10" t="s">
+        <v>113</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1462,8 +1466,8 @@
       <c r="C11" t="s">
         <v>106</v>
       </c>
-      <c r="D11">
-        <v>0</v>
+      <c r="D11" t="s">
+        <v>112</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1477,8 +1481,8 @@
       <c r="H11">
         <v>1000</v>
       </c>
-      <c r="I11" t="b">
-        <v>0</v>
+      <c r="I11" t="s">
+        <v>112</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1509,8 +1513,8 @@
       <c r="C12" t="s">
         <v>106</v>
       </c>
-      <c r="D12">
-        <v>0</v>
+      <c r="D12" t="s">
+        <v>112</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1524,8 +1528,8 @@
       <c r="H12">
         <v>4</v>
       </c>
-      <c r="I12" t="b">
-        <v>0</v>
+      <c r="I12" t="s">
+        <v>112</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1556,8 +1560,8 @@
       <c r="C13" t="s">
         <v>105</v>
       </c>
-      <c r="D13">
-        <v>0</v>
+      <c r="D13" t="s">
+        <v>112</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -1571,8 +1575,8 @@
       <c r="H13">
         <v>4</v>
       </c>
-      <c r="I13" t="b">
-        <v>1</v>
+      <c r="I13" t="s">
+        <v>113</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1603,8 +1607,8 @@
       <c r="C14" t="s">
         <v>105</v>
       </c>
-      <c r="D14">
-        <v>0</v>
+      <c r="D14" t="s">
+        <v>112</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1618,8 +1622,8 @@
       <c r="H14">
         <v>4</v>
       </c>
-      <c r="I14" t="b">
-        <v>1</v>
+      <c r="I14" t="s">
+        <v>113</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1650,8 +1654,8 @@
       <c r="C15" t="s">
         <v>106</v>
       </c>
-      <c r="D15">
-        <v>0</v>
+      <c r="D15" t="s">
+        <v>112</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -1665,8 +1669,8 @@
       <c r="H15">
         <v>4</v>
       </c>
-      <c r="I15" t="b">
-        <v>1</v>
+      <c r="I15" t="s">
+        <v>113</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1697,8 +1701,8 @@
       <c r="C16" t="s">
         <v>106</v>
       </c>
-      <c r="D16">
-        <v>0</v>
+      <c r="D16" t="s">
+        <v>112</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1712,8 +1716,8 @@
       <c r="H16">
         <v>1000</v>
       </c>
-      <c r="I16" t="b">
-        <v>0</v>
+      <c r="I16" t="s">
+        <v>112</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1744,8 +1748,8 @@
       <c r="C17" t="s">
         <v>106</v>
       </c>
-      <c r="D17">
-        <v>1</v>
+      <c r="D17" t="s">
+        <v>113</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1759,8 +1763,8 @@
       <c r="H17">
         <v>8</v>
       </c>
-      <c r="I17" t="b">
-        <v>1</v>
+      <c r="I17" t="s">
+        <v>113</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -1791,8 +1795,8 @@
       <c r="C18" t="s">
         <v>105</v>
       </c>
-      <c r="D18">
-        <v>1</v>
+      <c r="D18" t="s">
+        <v>113</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1806,8 +1810,8 @@
       <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" t="b">
-        <v>1</v>
+      <c r="I18" t="s">
+        <v>113</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1838,8 +1842,8 @@
       <c r="C19" t="s">
         <v>106</v>
       </c>
-      <c r="D19">
-        <v>1</v>
+      <c r="D19" t="s">
+        <v>113</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1853,8 +1857,8 @@
       <c r="H19">
         <v>11</v>
       </c>
-      <c r="I19" t="b">
-        <v>1</v>
+      <c r="I19" t="s">
+        <v>113</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1885,8 +1889,8 @@
       <c r="C20" t="s">
         <v>106</v>
       </c>
-      <c r="D20">
-        <v>1</v>
+      <c r="D20" t="s">
+        <v>113</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1900,8 +1904,8 @@
       <c r="H20">
         <v>11</v>
       </c>
-      <c r="I20" t="b">
-        <v>1</v>
+      <c r="I20" t="s">
+        <v>113</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1931,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
First attempt at merging the data input and solving parts
</commit_message>
<xml_diff>
--- a/sample_data/DataFile.xlsx
+++ b/sample_data/DataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-443" windowWidth="13680" windowHeight="10500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-443" windowWidth="13680" windowHeight="10500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="105">
   <si>
     <t>MICU_D</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>VAC</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>Resident_ID</t>
@@ -761,13 +758,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
@@ -799,7 +796,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Blue")</f>
@@ -811,7 +808,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Green")</f>
@@ -823,7 +820,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Orange")</f>
@@ -844,7 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -860,49 +857,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>79</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>81</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>82</v>
-      </c>
-      <c r="O1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
@@ -910,13 +907,13 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -931,7 +928,7 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -954,16 +951,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -978,7 +975,7 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1001,16 +998,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1025,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -1048,16 +1045,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1072,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1095,16 +1092,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1119,7 +1116,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1145,13 +1142,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1166,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1192,13 +1189,13 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1213,7 +1210,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1239,13 +1236,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1260,7 +1257,7 @@
         <v>1000</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1286,13 +1283,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1307,7 +1304,7 @@
         <v>1000</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1333,13 +1330,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1354,7 +1351,7 @@
         <v>1000</v>
       </c>
       <c r="I11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1380,13 +1377,13 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
         <v>101</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>102</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1401,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1427,13 +1424,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -1448,7 +1445,7 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1474,13 +1471,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1495,7 +1492,7 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1521,13 +1518,13 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -1542,7 +1539,7 @@
         <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1565,16 +1562,16 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1589,7 +1586,7 @@
         <v>1000</v>
       </c>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1615,13 +1612,13 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1636,7 +1633,7 @@
         <v>8</v>
       </c>
       <c r="I17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -1662,13 +1659,13 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1683,7 +1680,7 @@
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -1706,16 +1703,16 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1730,7 +1727,7 @@
         <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1759,10 +1756,10 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1777,7 +1774,7 @@
         <v>11</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -1807,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:BC46"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AC7" sqref="D2:BC58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1822,169 +1819,169 @@
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.5">
@@ -2907,8 +2904,8 @@
       <c r="AB7" s="2">
         <v>0</v>
       </c>
-      <c r="AC7" s="2" t="s">
-        <v>19</v>
+      <c r="AC7" s="2">
+        <v>0</v>
       </c>
       <c r="AD7" s="2">
         <v>7</v>
@@ -3038,8 +3035,8 @@
       <c r="P8" s="2">
         <v>4</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>19</v>
+      <c r="Q8" s="2">
+        <v>0</v>
       </c>
       <c r="R8" s="2">
         <v>0</v>
@@ -8755,8 +8752,8 @@
       <c r="AC42" s="2">
         <v>0</v>
       </c>
-      <c r="AD42" s="2" t="s">
-        <v>19</v>
+      <c r="AD42" s="2">
+        <v>0</v>
       </c>
       <c r="AE42" s="2">
         <v>7</v>
@@ -10860,17 +10857,17 @@
       <c r="G55" s="2">
         <v>0</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>19</v>
+      <c r="H55" s="2">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0</v>
+      </c>
+      <c r="J55" s="2">
+        <v>0</v>
+      </c>
+      <c r="K55" s="2">
+        <v>0</v>
       </c>
       <c r="L55" s="2">
         <v>7</v>
@@ -11542,10 +11539,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>16</v>
@@ -11554,7 +11551,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -11566,13 +11563,13 @@
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>18</v>

</xml_diff>